<commit_message>
Add missing 19-pin hdmi ffc to BOM
</commit_message>
<xml_diff>
--- a/full-bom.xlsx
+++ b/full-bom.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="193">
+  <si>
+    <t>Board</t>
+  </si>
   <si>
     <t>Reference</t>
   </si>
@@ -528,6 +531,15 @@
     <t>2073-05-08-D-0030-A-4-06-4-T-ND</t>
   </si>
   <si>
+    <t>CABLE FFC/FPC 19POS 0.5MM 3.98"</t>
+  </si>
+  <si>
+    <t>05-19-A-0101-A-4-06-4-T</t>
+  </si>
+  <si>
+    <t>2073-05-19-A-0101-A-4-06-4-T-ND</t>
+  </si>
+  <si>
     <t>CABLE ASSY PICOLOCK 5 POS 50MM</t>
   </si>
   <si>
@@ -537,7 +549,7 @@
     <t>Alternatively - crimp your own cables to reduce BOM cost</t>
   </si>
   <si>
-    <t>GC Controller Dongles</t>
+    <t>Controller Dongles</t>
   </si>
   <si>
     <t>GameCube extension cable</t>
@@ -961,21 +973,23 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -998,139 +1012,139 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4">
         <v>4.0</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="4">
         <v>4.0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="4">
         <v>5.0</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4">
         <v>4.0</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="4">
         <v>3.0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="4">
         <v>1.0</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="4">
         <v>4.0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="4">
         <v>1.0</v>
@@ -1139,16 +1153,16 @@
         <v>5.040500591E9</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="4">
         <v>1.0</v>
@@ -1157,16 +1171,16 @@
         <v>5.0348014E9</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="4">
         <v>1.0</v>
@@ -1175,16 +1189,16 @@
         <v>5.41020164E8</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D12" s="4">
         <v>1.0</v>
@@ -1193,16 +1207,16 @@
         <v>2.171790001E9</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D13" s="4">
         <v>1.0</v>
@@ -1211,34 +1225,34 @@
         <v>5.052781933E9</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D14" s="4">
         <v>1.0</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D15" s="4">
         <v>1.0</v>
@@ -1247,16 +1261,16 @@
         <v>5.033981892E9</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D16" s="4">
         <v>1.0</v>
@@ -1265,354 +1279,354 @@
         <v>5.0348008E9</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17" s="4">
         <v>1.0</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="4">
         <v>4.0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" s="4">
         <v>1.0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D20" s="4">
         <v>4.0</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D21" s="4">
         <v>1.0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D22" s="4">
         <v>1.0</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D23" s="4">
         <v>1.0</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D24" s="4">
         <v>2.0</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D25" s="4">
         <v>1.0</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D26" s="4">
         <v>3.0</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D27" s="4">
         <v>1.0</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D28" s="4">
         <v>4.0</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D29" s="4">
         <v>1.0</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D30" s="4">
         <v>1.0</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D31" s="4">
         <v>1.0</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D32" s="4">
         <v>1.0</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D33" s="4">
         <v>1.0</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D34" s="4">
         <v>1.0</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D35" s="8">
         <v>3.0</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="9"/>
@@ -1635,44 +1649,44 @@
     </row>
     <row r="36">
       <c r="B36" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D36" s="4">
         <v>2.0</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D37" s="4">
         <v>1.0</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D38" s="4">
         <v>1.0</v>
@@ -1681,62 +1695,62 @@
         <v>5.0348008E9</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D39" s="4">
         <v>3.0</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D40" s="4">
         <v>3.0</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D41" s="8">
         <v>1.0</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -1759,44 +1773,44 @@
     <row r="42">
       <c r="A42" s="1"/>
       <c r="C42" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
       <c r="F42" s="4"/>
       <c r="G42" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1"/>
       <c r="C43" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E43" s="12"/>
       <c r="G43" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D44" s="8">
         <v>1.0</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
@@ -1819,185 +1833,197 @@
     <row r="45">
       <c r="A45" s="1"/>
       <c r="C45" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D45" s="4">
         <v>1.0</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1"/>
       <c r="C46" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D46" s="4">
+        <v>168</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1"/>
+      <c r="C47" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" s="4">
         <v>1.0</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E47" s="5">
         <v>1.513205E8</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="D47" s="8">
+      <c r="F47" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D48" s="8">
         <v>4.0</v>
       </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
-      <c r="Q47" s="9"/>
-      <c r="R47" s="9"/>
-      <c r="S47" s="9"/>
-      <c r="T47" s="9"/>
-      <c r="U47" s="9"/>
-      <c r="V47" s="9"/>
-      <c r="W47" s="9"/>
-      <c r="X47" s="9"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="1"/>
-      <c r="C48" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D48" s="4">
+      <c r="E48" s="13"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="9"/>
+      <c r="V48" s="9"/>
+      <c r="W48" s="9"/>
+      <c r="X48" s="9"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="1"/>
+      <c r="C49" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D49" s="4">
         <v>4.0</v>
       </c>
-      <c r="E48" s="12"/>
-      <c r="G48" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="D49" s="8">
+      <c r="E49" s="12"/>
+      <c r="G49" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="8">
         <v>4.0</v>
       </c>
-      <c r="E49" s="13"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="9"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="9"/>
-      <c r="Q49" s="9"/>
-      <c r="R49" s="9"/>
-      <c r="S49" s="9"/>
-      <c r="T49" s="9"/>
-      <c r="U49" s="9"/>
-      <c r="V49" s="9"/>
-      <c r="W49" s="9"/>
-      <c r="X49" s="9"/>
-    </row>
-    <row r="50">
-      <c r="C50" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D50" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="E50" s="12"/>
-      <c r="G50" s="15" t="s">
-        <v>179</v>
-      </c>
+      <c r="E50" s="13"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="9"/>
+      <c r="V50" s="9"/>
+      <c r="W50" s="9"/>
+      <c r="X50" s="9"/>
     </row>
     <row r="51">
       <c r="C51" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D51" s="4">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="E51" s="12"/>
-      <c r="G51" s="6" t="s">
-        <v>181</v>
+      <c r="G51" s="15" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="52">
       <c r="C52" s="5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D52" s="4">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="E52" s="12"/>
       <c r="G52" s="6" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="53">
       <c r="C53" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D53" s="4">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="E53" s="12"/>
-      <c r="G53" s="15" t="s">
-        <v>185</v>
+      <c r="G53" s="6" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="54">
       <c r="C54" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D54" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E54" s="12"/>
+      <c r="G54" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="C55" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D55" s="4">
         <v>1.0</v>
       </c>
-      <c r="E54" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="C55" s="12"/>
-      <c r="E55" s="12"/>
+      <c r="E55" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="56">
       <c r="C56" s="12"/>
@@ -5810,19 +5836,23 @@
     <row r="1008">
       <c r="C1008" s="12"/>
       <c r="E1008" s="12"/>
+    </row>
+    <row r="1009">
+      <c r="C1009" s="12"/>
+      <c r="E1009" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G30"/>
     <hyperlink r:id="rId2" ref="G41"/>
     <hyperlink r:id="rId3" ref="G42"/>
-    <hyperlink r:id="rId4" ref="G47"/>
-    <hyperlink r:id="rId5" ref="G48"/>
-    <hyperlink r:id="rId6" ref="G49"/>
-    <hyperlink r:id="rId7" ref="G50"/>
-    <hyperlink r:id="rId8" ref="G51"/>
-    <hyperlink r:id="rId9" ref="G52"/>
-    <hyperlink r:id="rId10" ref="G53"/>
+    <hyperlink r:id="rId4" ref="G48"/>
+    <hyperlink r:id="rId5" ref="G49"/>
+    <hyperlink r:id="rId6" ref="G50"/>
+    <hyperlink r:id="rId7" ref="G51"/>
+    <hyperlink r:id="rId8" ref="G52"/>
+    <hyperlink r:id="rId9" ref="G53"/>
+    <hyperlink r:id="rId10" ref="G54"/>
   </hyperlinks>
   <drawing r:id="rId11"/>
 </worksheet>

</xml_diff>